<commit_message>
Se modificar el objeto de usuario temporal, debido a que no estaba actualizando los datos
</commit_message>
<xml_diff>
--- a/PLANTILLA_CARGUE.xlsx
+++ b/PLANTILLA_CARGUE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="CARTERA_ELECTRO" sheetId="1" r:id="rId1"/>
@@ -53,12 +53,6 @@
     <t>FVC-13759-2</t>
   </si>
   <si>
-    <t>JOSE</t>
-  </si>
-  <si>
-    <t>JULIAN</t>
-  </si>
-  <si>
     <t>DURAN</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>9713RESTREPO@GMAIL.COM</t>
   </si>
   <si>
-    <t>9621diegomania@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">903.mauricio@gmail.com </t>
   </si>
   <si>
@@ -350,6 +341,15 @@
   </si>
   <si>
     <t>95AGUIRRE@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>dluis_04@hotmail.com</t>
+  </si>
+  <si>
+    <t>JULIAN - MODIFICADO</t>
+  </si>
+  <si>
+    <t>JOSE - MODIFICADO</t>
   </si>
 </sst>
 </file>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1216,64 +1216,64 @@
   <sheetData>
     <row r="1" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1335,7 +1335,7 @@
         <v>3206352198</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1364,25 +1364,25 @@
         <v>10006171</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="P3" s="1">
         <v>3209100533</v>
@@ -1396,13 +1396,13 @@
       <c r="S3" s="1">
         <v>3209100533</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>90</v>
+      <c r="T3" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -1426,25 +1426,25 @@
         <v>10006924</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="P4" s="1">
         <v>3188535637</v>
@@ -1459,12 +1459,12 @@
         <v>0</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1488,25 +1488,25 @@
         <v>10006924</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="P5" s="1">
         <v>3188535637</v>
@@ -1521,12 +1521,12 @@
         <v>0</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -1550,25 +1550,25 @@
         <v>1000870241</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P6" s="1">
         <v>3226610364</v>
@@ -1583,12 +1583,12 @@
         <v>3166935070</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1612,25 +1612,25 @@
         <v>1000930458</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="O7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P7" s="1">
         <v>3127102010</v>
@@ -1645,12 +1645,12 @@
         <v>3127102010</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -1674,19 +1674,19 @@
         <v>10012624</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>6</v>
@@ -1707,12 +1707,12 @@
         <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -1736,25 +1736,25 @@
         <v>1001283419</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P9" s="1">
         <v>3156609902</v>
@@ -1769,12 +1769,12 @@
         <v>3156609902</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1798,19 +1798,19 @@
         <v>10013708</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>6</v>
@@ -1831,12 +1831,12 @@
         <v>3137382247</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1860,25 +1860,25 @@
         <v>10013715</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="P11" s="1">
         <v>3215891216</v>
@@ -1893,12 +1893,12 @@
         <v>3108488989</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1922,25 +1922,25 @@
         <v>10013715</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="P12" s="1">
         <v>3215891216</v>
@@ -1955,12 +1955,12 @@
         <v>3215891216</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1984,25 +1984,25 @@
         <v>10014154</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="N13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P13" s="1">
         <v>3148029540</v>
@@ -2017,12 +2017,12 @@
         <v>2</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -2046,19 +2046,19 @@
         <v>10014939</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>6</v>
@@ -2079,7 +2079,7 @@
         <v>22</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2089,6 +2089,7 @@
     <hyperlink ref="T5" r:id="rId3"/>
     <hyperlink ref="T12" r:id="rId4"/>
     <hyperlink ref="T13" r:id="rId5"/>
+    <hyperlink ref="T3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se modififica la plantilla cargue para pruebas de actualizacion de datos
</commit_message>
<xml_diff>
--- a/PLANTILLA_CARGUE.xlsx
+++ b/PLANTILLA_CARGUE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="CARTERA_ELECTRO" sheetId="1" r:id="rId1"/>
@@ -53,18 +53,6 @@
     <t>FVC-13759-2</t>
   </si>
   <si>
-    <t>JOSE</t>
-  </si>
-  <si>
-    <t>JULIAN</t>
-  </si>
-  <si>
-    <t>DURAN</t>
-  </si>
-  <si>
-    <t>CASTRO</t>
-  </si>
-  <si>
     <t>MZ 28 CA 39 EL REMANZO VILLA SANTANA</t>
   </si>
   <si>
@@ -316,9 +304,6 @@
     <t>9713RESTREPO@GMAIL.COM</t>
   </si>
   <si>
-    <t>9621diegomania@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">903.mauricio@gmail.com </t>
   </si>
   <si>
@@ -350,6 +335,21 @@
   </si>
   <si>
     <t>95AGUIRRE@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>JOSE - MODIFICADO</t>
+  </si>
+  <si>
+    <t>JULIAN - MODIFICADO</t>
+  </si>
+  <si>
+    <t>DURAN - MODIFICADO</t>
+  </si>
+  <si>
+    <t>CASTRO - MODIFICADO</t>
+  </si>
+  <si>
+    <t>dluis_04@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1216,64 +1216,64 @@
   <sheetData>
     <row r="1" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="H1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1335,7 +1335,7 @@
         <v>3206352198</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1364,19 +1364,19 @@
         <v>10006171</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>6</v>
@@ -1396,13 +1396,13 @@
       <c r="S3" s="1">
         <v>3209100533</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>90</v>
+      <c r="T3" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -1426,25 +1426,25 @@
         <v>10006924</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="P4" s="1">
         <v>3188535637</v>
@@ -1459,12 +1459,12 @@
         <v>0</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1488,25 +1488,25 @@
         <v>10006924</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="P5" s="1">
         <v>3188535637</v>
@@ -1521,12 +1521,12 @@
         <v>0</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -1550,25 +1550,25 @@
         <v>1000870241</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P6" s="1">
         <v>3226610364</v>
@@ -1583,12 +1583,12 @@
         <v>3166935070</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1612,25 +1612,25 @@
         <v>1000930458</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P7" s="1">
         <v>3127102010</v>
@@ -1645,12 +1645,12 @@
         <v>3127102010</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -1674,19 +1674,19 @@
         <v>10012624</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>6</v>
@@ -1707,12 +1707,12 @@
         <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -1736,25 +1736,25 @@
         <v>1001283419</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P9" s="1">
         <v>3156609902</v>
@@ -1769,12 +1769,12 @@
         <v>3156609902</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1798,19 +1798,19 @@
         <v>10013708</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>6</v>
@@ -1831,12 +1831,12 @@
         <v>3137382247</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1860,25 +1860,25 @@
         <v>10013715</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="P11" s="1">
         <v>3215891216</v>
@@ -1893,12 +1893,12 @@
         <v>3108488989</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1922,25 +1922,25 @@
         <v>10013715</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="P12" s="1">
         <v>3215891216</v>
@@ -1955,12 +1955,12 @@
         <v>3215891216</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1984,25 +1984,25 @@
         <v>10014154</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="N13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P13" s="1">
         <v>3148029540</v>
@@ -2017,12 +2017,12 @@
         <v>2</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -2046,19 +2046,19 @@
         <v>10014939</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>6</v>
@@ -2079,7 +2079,7 @@
         <v>22</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2089,6 +2089,7 @@
     <hyperlink ref="T5" r:id="rId3"/>
     <hyperlink ref="T12" r:id="rId4"/>
     <hyperlink ref="T13" r:id="rId5"/>
+    <hyperlink ref="T3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>